<commit_message>
add headless browser testing
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Brand</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Samsung Selected</t>
+  </si>
+  <si>
+    <t>First Product Selected</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>